<commit_message>
Completed charger board and BOM.
</commit_message>
<xml_diff>
--- a/RTx_Main_Power/RTxChargerBOM.xlsx
+++ b/RTx_Main_Power/RTxChargerBOM.xlsx
@@ -9,12 +9,15 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$B$2:$J$2</definedName>
+  </definedNames>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="47">
   <si>
     <t>Qty</t>
   </si>
@@ -109,12 +112,6 @@
     <t>311-10.0KFRCT-ND</t>
   </si>
   <si>
-    <t>Using 232k resistor which is closest standard size</t>
-  </si>
-  <si>
-    <t>311-232KFRCT-ND</t>
-  </si>
-  <si>
     <t>497-4420-5-ND</t>
   </si>
   <si>
@@ -125,6 +122,42 @@
   </si>
   <si>
     <t>Digi-Key Part Number</t>
+  </si>
+  <si>
+    <t>ATO_FUSEHOLDER</t>
+  </si>
+  <si>
+    <t>FUSEATO_FUSEHOLDER</t>
+  </si>
+  <si>
+    <t>ATO_BLADE_FUSE</t>
+  </si>
+  <si>
+    <t>FUSE</t>
+  </si>
+  <si>
+    <t>G4W-1114P-US-TV8-HP</t>
+  </si>
+  <si>
+    <t>RELAY</t>
+  </si>
+  <si>
+    <t>Z962-ND</t>
+  </si>
+  <si>
+    <t>F5187-ND</t>
+  </si>
+  <si>
+    <t>Fuse Holder</t>
+  </si>
+  <si>
+    <t>SPST Relay</t>
+  </si>
+  <si>
+    <t>Using 226k resistor which is a standard size down</t>
+  </si>
+  <si>
+    <t>311-226KFRCT-ND</t>
   </si>
 </sst>
 </file>
@@ -508,19 +541,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B1:J9"/>
+  <dimension ref="B1:J11"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="1.5703125" style="2" customWidth="1"/>
-    <col min="2" max="2" width="9.140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="21.85546875" style="2" customWidth="1"/>
+    <col min="2" max="2" width="14.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="25.42578125" style="2" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="43.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="13.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.28515625" style="2" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="21.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="21.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="21.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.5703125" style="2" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="10.28515625" style="2" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="33.5703125" style="2" bestFit="1" customWidth="1"/>
     <col min="11" max="16384" width="9.140625" style="2"/>
@@ -532,7 +566,7 @@
         <v>26</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D2" s="3" t="s">
         <v>27</v>
@@ -640,10 +674,10 @@
         <v>3</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>32</v>
+        <v>46</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>31</v>
+        <v>45</v>
       </c>
       <c r="E6" s="6" t="s">
         <v>14</v>
@@ -669,7 +703,7 @@
         <v>3</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D7" s="5"/>
       <c r="E7" s="6" t="s">
@@ -696,7 +730,7 @@
         <v>3</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="D8" s="5"/>
       <c r="E8" s="6" t="s">
@@ -723,7 +757,7 @@
         <v>3</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D9" s="5"/>
       <c r="E9" s="6" t="s">
@@ -745,7 +779,62 @@
         <v>25</v>
       </c>
     </row>
+    <row r="10" spans="2:10">
+      <c r="B10" s="5">
+        <v>3</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="D10" s="5"/>
+      <c r="E10" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="F10" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="G10" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="H10" s="5">
+        <v>1</v>
+      </c>
+      <c r="I10" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="J10" s="6" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="11" spans="2:10">
+      <c r="B11" s="5">
+        <v>3</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="D11" s="5"/>
+      <c r="E11" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="F11" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="G11" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="H11" s="5">
+        <v>1</v>
+      </c>
+      <c r="I11" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="J11" s="6" t="s">
+        <v>44</v>
+      </c>
+    </row>
   </sheetData>
+  <autoFilter ref="B2:J2"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Added panel-mount D-Sub to BOM.
</commit_message>
<xml_diff>
--- a/RTx_Main_Power/RTxChargerBOM.xlsx
+++ b/RTx_Main_Power/RTxChargerBOM.xlsx
@@ -10,14 +10,14 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$B$2:$J$2</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$I$1</definedName>
   </definedNames>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="49">
   <si>
     <t>Qty</t>
   </si>
@@ -158,6 +158,12 @@
   </si>
   <si>
     <t>311-226KFRCT-ND</t>
+  </si>
+  <si>
+    <t>AE10114-ND</t>
+  </si>
+  <si>
+    <t>D-Sub for enclosure</t>
   </si>
 </sst>
 </file>
@@ -229,22 +235,22 @@
   </cellStyleXfs>
   <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
@@ -541,300 +547,317 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B1:J11"/>
+  <dimension ref="A1:I11"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="C16" sqref="C16"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="1.5703125" style="2" customWidth="1"/>
-    <col min="2" max="2" width="14.28515625" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="25.42578125" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="43.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="21.5703125" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="21.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="21.5703125" style="2" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="8.5703125" style="2" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.28515625" style="2" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="33.5703125" style="2" bestFit="1" customWidth="1"/>
-    <col min="11" max="16384" width="9.140625" style="2"/>
+    <col min="1" max="1" width="14.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="43.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="21.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="21.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="33.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:10" ht="8.25" customHeight="1"/>
-    <row r="2" spans="2:10" s="1" customFormat="1" ht="27.75" customHeight="1">
-      <c r="B2" s="3" t="s">
+    <row r="1" spans="1:9" s="4" customFormat="1" ht="27.75" customHeight="1">
+      <c r="A1" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="B1" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="C1" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="E2" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="F2" s="4" t="s">
+      <c r="D1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="G2" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="H2" s="3" t="s">
+      <c r="F1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="I2" s="4" t="s">
+      <c r="H1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="J2" s="4" t="s">
+      <c r="I1" s="3" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="2:10">
-      <c r="B3" s="5">
-        <v>3</v>
-      </c>
-      <c r="C3" s="5" t="s">
+    <row r="2" spans="1:9">
+      <c r="A2" s="5">
+        <v>3</v>
+      </c>
+      <c r="B2" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="D3" s="5"/>
-      <c r="E3" s="6">
+      <c r="C2" s="5"/>
+      <c r="D2" s="6">
         <v>0</v>
       </c>
+      <c r="E2" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="F2" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="G2" s="5">
+        <v>1</v>
+      </c>
+      <c r="H2" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="I2" s="6" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9">
+      <c r="A3" s="5">
+        <v>3</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="C3" s="5"/>
+      <c r="D3" s="6">
+        <v>10</v>
+      </c>
+      <c r="E3" s="6" t="s">
+        <v>10</v>
+      </c>
       <c r="F3" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="G3" s="5">
+        <v>1</v>
+      </c>
+      <c r="H3" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="I3" s="6"/>
+    </row>
+    <row r="4" spans="1:9">
+      <c r="A4" s="5">
+        <v>3</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="C4" s="5"/>
+      <c r="D4" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="E4" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="G3" s="6" t="s">
+      <c r="F4" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="H3" s="5">
-        <v>1</v>
-      </c>
-      <c r="I3" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="J3" s="6" t="s">
+      <c r="G4" s="5">
+        <v>1</v>
+      </c>
+      <c r="H4" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="I4" s="6" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="2:10">
-      <c r="B4" s="5">
-        <v>3</v>
-      </c>
-      <c r="C4" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="D4" s="5"/>
-      <c r="E4" s="6">
-        <v>10</v>
-      </c>
-      <c r="F4" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="G4" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="H4" s="5">
-        <v>1</v>
-      </c>
-      <c r="I4" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="J4" s="6"/>
-    </row>
-    <row r="5" spans="2:10">
-      <c r="B5" s="5">
-        <v>3</v>
+    <row r="5" spans="1:9">
+      <c r="A5" s="5">
+        <v>3</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>46</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="D5" s="5"/>
+        <v>45</v>
+      </c>
+      <c r="D5" s="6" t="s">
+        <v>14</v>
+      </c>
       <c r="E5" s="6" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="F5" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="G5" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="H5" s="5">
-        <v>1</v>
+      <c r="G5" s="5">
+        <v>1</v>
+      </c>
+      <c r="H5" s="6" t="s">
+        <v>15</v>
       </c>
       <c r="I5" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="J5" s="6" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="2:10">
-      <c r="B6" s="5">
-        <v>3</v>
-      </c>
-      <c r="C6" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="D6" s="5" t="s">
-        <v>45</v>
+    <row r="6" spans="1:9">
+      <c r="A6" s="5">
+        <v>3</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="C6" s="5"/>
+      <c r="D6" s="6" t="s">
+        <v>16</v>
       </c>
       <c r="E6" s="6" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="F6" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="G6" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="H6" s="5">
-        <v>1</v>
+        <v>17</v>
+      </c>
+      <c r="G6" s="5">
+        <v>1</v>
+      </c>
+      <c r="H6" s="6" t="s">
+        <v>18</v>
       </c>
       <c r="I6" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="J6" s="6" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="7" spans="2:10">
-      <c r="B7" s="5">
-        <v>3</v>
-      </c>
-      <c r="C7" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="D7" s="5"/>
+        <v>19</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9">
+      <c r="A7" s="5">
+        <v>3</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="C7" s="5"/>
+      <c r="D7" s="6" t="s">
+        <v>20</v>
+      </c>
       <c r="E7" s="6" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="F7" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="G7" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="H7" s="5">
-        <v>1</v>
+        <v>21</v>
+      </c>
+      <c r="G7" s="5">
+        <v>1</v>
+      </c>
+      <c r="H7" s="6" t="s">
+        <v>22</v>
       </c>
       <c r="I7" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="J7" s="6" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="8" spans="2:10">
-      <c r="B8" s="5">
-        <v>3</v>
-      </c>
-      <c r="C8" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="D8" s="5"/>
+        <v>23</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9">
+      <c r="A8" s="5">
+        <v>3</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="C8" s="5"/>
+      <c r="D8" s="6" t="s">
+        <v>24</v>
+      </c>
       <c r="E8" s="6" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="F8" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="G8" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="H8" s="5">
-        <v>1</v>
+        <v>24</v>
+      </c>
+      <c r="G8" s="5">
+        <v>1</v>
+      </c>
+      <c r="H8" s="6" t="s">
+        <v>25</v>
       </c>
       <c r="I8" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="J8" s="6" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="9" spans="2:10">
-      <c r="B9" s="5">
-        <v>3</v>
-      </c>
-      <c r="C9" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="D9" s="5"/>
+        <v>25</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9">
+      <c r="A9" s="5">
+        <v>3</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="C9" s="5"/>
+      <c r="D9" s="6" t="s">
+        <v>35</v>
+      </c>
       <c r="E9" s="6" t="s">
-        <v>24</v>
+        <v>36</v>
       </c>
       <c r="F9" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="G9" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="H9" s="5">
-        <v>1</v>
+        <v>37</v>
+      </c>
+      <c r="G9" s="5">
+        <v>1</v>
+      </c>
+      <c r="H9" s="6" t="s">
+        <v>38</v>
       </c>
       <c r="I9" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="J9" s="6" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="10" spans="2:10">
-      <c r="B10" s="5">
-        <v>3</v>
-      </c>
-      <c r="C10" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="D10" s="5"/>
+        <v>43</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9">
+      <c r="A10" s="5">
+        <v>3</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="C10" s="5"/>
+      <c r="D10" s="6" t="s">
+        <v>39</v>
+      </c>
       <c r="E10" s="6" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="F10" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="G10" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="H10" s="5">
-        <v>1</v>
+        <v>39</v>
+      </c>
+      <c r="G10" s="5">
+        <v>1</v>
+      </c>
+      <c r="H10" s="6" t="s">
+        <v>40</v>
       </c>
       <c r="I10" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="J10" s="6" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="11" spans="2:10">
-      <c r="B11" s="5">
-        <v>3</v>
-      </c>
-      <c r="C11" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="D11" s="5"/>
+        <v>44</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9">
+      <c r="A11" s="6">
+        <v>1</v>
+      </c>
+      <c r="B11" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="C11" s="6"/>
+      <c r="D11" s="6"/>
       <c r="E11" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="F11" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="G11" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="H11" s="5">
-        <v>1</v>
-      </c>
-      <c r="I11" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="J11" s="6" t="s">
-        <v>44</v>
-      </c>
+        <v>48</v>
+      </c>
+      <c r="F11" s="6"/>
+      <c r="G11" s="6"/>
+      <c r="H11" s="6"/>
+      <c r="I11" s="6"/>
     </row>
   </sheetData>
-  <autoFilter ref="B2:J2"/>
+  <autoFilter ref="A1:I1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>